<commit_message>
analisis distancias por Radar y por Estela
</commit_message>
<xml_diff>
--- a/WinForms/Excelp3/2305_02_dep_lebl.xlsx
+++ b/WinForms/Excelp3/2305_02_dep_lebl.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://enaire-my.sharepoint.com/personal/aprades_enaire_es/Documents/Docs/Mi Universidad/2018-PGTA/P3_new/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proyecto2_v1.4\Proyecto2_v1.4\WinForms\Excelp3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="8_{03440527-6269-48D3-8FEB-CD36B4438294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7CF83CEB-417A-44D1-9D93-76E2D650E6AE}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C73691D-CE06-44D5-9A71-3C5CA0B47138}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B756B1F3-1E48-456A-9F1E-1618740E9DEF}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="15705" windowHeight="15585" xr2:uid="{B756B1F3-1E48-456A-9F1E-1618740E9DEF}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2684" uniqueCount="651">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2684" uniqueCount="664">
   <si>
     <t>id</t>
   </si>
@@ -1992,6 +1992,45 @@
   </si>
   <si>
     <t>LOTOS3R</t>
+  </si>
+  <si>
+    <t>NATPI2R</t>
+  </si>
+  <si>
+    <t>DIPES1R</t>
+  </si>
+  <si>
+    <t>LAPRA4R</t>
+  </si>
+  <si>
+    <t>LOTOS6Q</t>
+  </si>
+  <si>
+    <t>LOBAR7Q</t>
+  </si>
+  <si>
+    <t>GRAUS6Q</t>
+  </si>
+  <si>
+    <t>SENIA6Q</t>
+  </si>
+  <si>
+    <t>NATPI3Q</t>
+  </si>
+  <si>
+    <t>AGENA6Q</t>
+  </si>
+  <si>
+    <t>DALIN5Q</t>
+  </si>
+  <si>
+    <t>DUNES6Q</t>
+  </si>
+  <si>
+    <t>LAPRA6Q</t>
+  </si>
+  <si>
+    <t>DIPES2Q</t>
   </si>
 </sst>
 </file>
@@ -2053,10 +2092,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2358,17 +2393,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF98AAC8-0A8C-4C65-A83E-F22551017F80}">
   <dimension ref="A1:H447"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B123" sqref="B123"/>
+    <sheetView tabSelected="1" topLeftCell="B163" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F448" sqref="F448"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="21.109375" customWidth="1"/>
-    <col min="4" max="4" width="97.109375" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" customWidth="1"/>
+    <col min="4" max="4" width="97.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2394,7 +2429,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>458</v>
       </c>
@@ -2420,7 +2455,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>459</v>
       </c>
@@ -2446,7 +2481,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>460</v>
       </c>
@@ -2472,7 +2507,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>461</v>
       </c>
@@ -2498,7 +2533,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>462</v>
       </c>
@@ -2524,7 +2559,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>463</v>
       </c>
@@ -2550,7 +2585,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>464</v>
       </c>
@@ -2576,7 +2611,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>465</v>
       </c>
@@ -2602,7 +2637,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>466</v>
       </c>
@@ -2628,7 +2663,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>467</v>
       </c>
@@ -2648,13 +2683,13 @@
         <v>35</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>36</v>
+        <v>650</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>468</v>
       </c>
@@ -2674,13 +2709,13 @@
         <v>11</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>36</v>
+        <v>651</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>469</v>
       </c>
@@ -2700,13 +2735,13 @@
         <v>11</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>470</v>
       </c>
@@ -2726,13 +2761,13 @@
         <v>11</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>36</v>
+        <v>652</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>471</v>
       </c>
@@ -2758,7 +2793,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>472</v>
       </c>
@@ -2778,13 +2813,13 @@
         <v>11</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>36</v>
+        <v>653</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>473</v>
       </c>
@@ -2804,13 +2839,13 @@
         <v>11</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>474</v>
       </c>
@@ -2830,13 +2865,13 @@
         <v>11</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>36</v>
+        <v>650</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>475</v>
       </c>
@@ -2856,13 +2891,13 @@
         <v>11</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>476</v>
       </c>
@@ -2882,13 +2917,13 @@
         <v>11</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>477</v>
       </c>
@@ -2914,7 +2949,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>478</v>
       </c>
@@ -2940,7 +2975,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>479</v>
       </c>
@@ -2966,7 +3001,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>480</v>
       </c>
@@ -2992,7 +3027,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>481</v>
       </c>
@@ -3018,7 +3053,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>482</v>
       </c>
@@ -3044,7 +3079,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>483</v>
       </c>
@@ -3064,13 +3099,13 @@
         <v>11</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>36</v>
+        <v>654</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>484</v>
       </c>
@@ -3096,7 +3131,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>485</v>
       </c>
@@ -3122,7 +3157,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>486</v>
       </c>
@@ -3148,7 +3183,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>487</v>
       </c>
@@ -3174,7 +3209,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>488</v>
       </c>
@@ -3200,7 +3235,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>489</v>
       </c>
@@ -3226,7 +3261,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>490</v>
       </c>
@@ -3252,7 +3287,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>491</v>
       </c>
@@ -3278,7 +3313,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>492</v>
       </c>
@@ -3304,7 +3339,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>493</v>
       </c>
@@ -3330,7 +3365,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>494</v>
       </c>
@@ -3356,7 +3391,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>495</v>
       </c>
@@ -3382,7 +3417,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>496</v>
       </c>
@@ -3408,7 +3443,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>497</v>
       </c>
@@ -3434,7 +3469,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>498</v>
       </c>
@@ -3460,7 +3495,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>499</v>
       </c>
@@ -3486,7 +3521,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>500</v>
       </c>
@@ -3512,7 +3547,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>501</v>
       </c>
@@ -3538,7 +3573,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>502</v>
       </c>
@@ -3564,7 +3599,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>503</v>
       </c>
@@ -3590,7 +3625,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>504</v>
       </c>
@@ -3616,7 +3651,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>505</v>
       </c>
@@ -3642,7 +3677,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>506</v>
       </c>
@@ -3668,7 +3703,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>507</v>
       </c>
@@ -3694,7 +3729,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>508</v>
       </c>
@@ -3720,7 +3755,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>509</v>
       </c>
@@ -3746,7 +3781,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>510</v>
       </c>
@@ -3772,7 +3807,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>511</v>
       </c>
@@ -3798,7 +3833,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>512</v>
       </c>
@@ -3824,7 +3859,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>513</v>
       </c>
@@ -3850,7 +3885,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>514</v>
       </c>
@@ -3876,7 +3911,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>515</v>
       </c>
@@ -3902,7 +3937,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>516</v>
       </c>
@@ -3928,7 +3963,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>517</v>
       </c>
@@ -3954,7 +3989,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>518</v>
       </c>
@@ -3980,7 +4015,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>519</v>
       </c>
@@ -4006,7 +4041,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>520</v>
       </c>
@@ -4032,7 +4067,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>521</v>
       </c>
@@ -4058,7 +4093,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>522</v>
       </c>
@@ -4084,7 +4119,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>523</v>
       </c>
@@ -4110,7 +4145,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>524</v>
       </c>
@@ -4136,7 +4171,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>525</v>
       </c>
@@ -4162,7 +4197,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>526</v>
       </c>
@@ -4188,7 +4223,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>527</v>
       </c>
@@ -4214,7 +4249,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>528</v>
       </c>
@@ -4240,7 +4275,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>529</v>
       </c>
@@ -4266,7 +4301,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>530</v>
       </c>
@@ -4292,7 +4327,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>531</v>
       </c>
@@ -4318,7 +4353,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>532</v>
       </c>
@@ -4344,7 +4379,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>533</v>
       </c>
@@ -4370,7 +4405,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>534</v>
       </c>
@@ -4396,7 +4431,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>535</v>
       </c>
@@ -4422,7 +4457,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>536</v>
       </c>
@@ -4448,7 +4483,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>537</v>
       </c>
@@ -4474,7 +4509,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>538</v>
       </c>
@@ -4500,7 +4535,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>539</v>
       </c>
@@ -4526,7 +4561,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>540</v>
       </c>
@@ -4552,7 +4587,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>541</v>
       </c>
@@ -4578,7 +4613,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>542</v>
       </c>
@@ -4598,13 +4633,13 @@
         <v>11</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>36</v>
+        <v>655</v>
       </c>
       <c r="H86" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>543</v>
       </c>
@@ -4630,7 +4665,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>544</v>
       </c>
@@ -4656,7 +4691,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>545</v>
       </c>
@@ -4682,7 +4717,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>546</v>
       </c>
@@ -4708,7 +4743,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>547</v>
       </c>
@@ -4734,7 +4769,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>548</v>
       </c>
@@ -4760,7 +4795,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>549</v>
       </c>
@@ -4786,7 +4821,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>550</v>
       </c>
@@ -4806,13 +4841,13 @@
         <v>11</v>
       </c>
       <c r="G94" s="1" t="s">
-        <v>36</v>
+        <v>655</v>
       </c>
       <c r="H94" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>551</v>
       </c>
@@ -4838,7 +4873,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>552</v>
       </c>
@@ -4864,7 +4899,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>553</v>
       </c>
@@ -4884,13 +4919,13 @@
         <v>11</v>
       </c>
       <c r="G97" s="1" t="s">
-        <v>36</v>
+        <v>656</v>
       </c>
       <c r="H97" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>554</v>
       </c>
@@ -4916,7 +4951,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>555</v>
       </c>
@@ -4942,7 +4977,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>556</v>
       </c>
@@ -4968,7 +5003,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>557</v>
       </c>
@@ -4994,7 +5029,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>558</v>
       </c>
@@ -5014,13 +5049,13 @@
         <v>11</v>
       </c>
       <c r="G102" s="1" t="s">
-        <v>36</v>
+        <v>657</v>
       </c>
       <c r="H102" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>559</v>
       </c>
@@ -5040,13 +5075,13 @@
         <v>11</v>
       </c>
       <c r="G103" s="1" t="s">
-        <v>36</v>
+        <v>658</v>
       </c>
       <c r="H103" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>560</v>
       </c>
@@ -5072,7 +5107,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>561</v>
       </c>
@@ -5098,7 +5133,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>562</v>
       </c>
@@ -5118,13 +5153,13 @@
         <v>11</v>
       </c>
       <c r="G106" s="1" t="s">
-        <v>36</v>
+        <v>656</v>
       </c>
       <c r="H106" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>563</v>
       </c>
@@ -5150,7 +5185,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>564</v>
       </c>
@@ -5176,7 +5211,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>565</v>
       </c>
@@ -5202,7 +5237,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>566</v>
       </c>
@@ -5228,7 +5263,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>567</v>
       </c>
@@ -5254,7 +5289,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>568</v>
       </c>
@@ -5280,7 +5315,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>569</v>
       </c>
@@ -5306,7 +5341,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>570</v>
       </c>
@@ -5332,7 +5367,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>571</v>
       </c>
@@ -5358,7 +5393,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>572</v>
       </c>
@@ -5384,7 +5419,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>573</v>
       </c>
@@ -5410,7 +5445,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>574</v>
       </c>
@@ -5436,7 +5471,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>575</v>
       </c>
@@ -5462,7 +5497,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>576</v>
       </c>
@@ -5488,7 +5523,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>577</v>
       </c>
@@ -5514,7 +5549,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>578</v>
       </c>
@@ -5540,7 +5575,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>579</v>
       </c>
@@ -5566,7 +5601,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>580</v>
       </c>
@@ -5592,7 +5627,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>581</v>
       </c>
@@ -5618,7 +5653,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>582</v>
       </c>
@@ -5644,7 +5679,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>583</v>
       </c>
@@ -5670,7 +5705,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>584</v>
       </c>
@@ -5696,7 +5731,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>585</v>
       </c>
@@ -5722,7 +5757,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>586</v>
       </c>
@@ -5748,7 +5783,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>587</v>
       </c>
@@ -5774,7 +5809,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>588</v>
       </c>
@@ -5800,7 +5835,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>589</v>
       </c>
@@ -5826,7 +5861,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>590</v>
       </c>
@@ -5852,7 +5887,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>591</v>
       </c>
@@ -5878,7 +5913,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>592</v>
       </c>
@@ -5904,7 +5939,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>593</v>
       </c>
@@ -5930,7 +5965,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>594</v>
       </c>
@@ -5956,7 +5991,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>595</v>
       </c>
@@ -5982,7 +6017,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>596</v>
       </c>
@@ -6008,7 +6043,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>597</v>
       </c>
@@ -6034,7 +6069,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>598</v>
       </c>
@@ -6060,7 +6095,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>599</v>
       </c>
@@ -6086,7 +6121,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>600</v>
       </c>
@@ -6106,13 +6141,13 @@
         <v>11</v>
       </c>
       <c r="G144" s="1" t="s">
-        <v>36</v>
+        <v>659</v>
       </c>
       <c r="H144" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>601</v>
       </c>
@@ -6138,7 +6173,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>602</v>
       </c>
@@ -6164,7 +6199,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>603</v>
       </c>
@@ -6190,7 +6225,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>604</v>
       </c>
@@ -6216,7 +6251,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>605</v>
       </c>
@@ -6242,7 +6277,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>606</v>
       </c>
@@ -6268,7 +6303,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>607</v>
       </c>
@@ -6294,7 +6329,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>608</v>
       </c>
@@ -6320,7 +6355,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>609</v>
       </c>
@@ -6346,7 +6381,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>610</v>
       </c>
@@ -6372,7 +6407,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>611</v>
       </c>
@@ -6398,7 +6433,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>612</v>
       </c>
@@ -6424,7 +6459,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>613</v>
       </c>
@@ -6450,7 +6485,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>614</v>
       </c>
@@ -6476,7 +6511,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>615</v>
       </c>
@@ -6502,7 +6537,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>616</v>
       </c>
@@ -6528,7 +6563,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>617</v>
       </c>
@@ -6554,7 +6589,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>618</v>
       </c>
@@ -6580,7 +6615,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>619</v>
       </c>
@@ -6606,7 +6641,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>620</v>
       </c>
@@ -6632,7 +6667,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>621</v>
       </c>
@@ -6658,7 +6693,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>622</v>
       </c>
@@ -6684,7 +6719,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>623</v>
       </c>
@@ -6710,7 +6745,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>624</v>
       </c>
@@ -6736,7 +6771,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>625</v>
       </c>
@@ -6762,7 +6797,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>626</v>
       </c>
@@ -6788,7 +6823,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>627</v>
       </c>
@@ -6814,7 +6849,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>628</v>
       </c>
@@ -6840,7 +6875,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>629</v>
       </c>
@@ -6866,7 +6901,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>630</v>
       </c>
@@ -6892,7 +6927,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>631</v>
       </c>
@@ -6918,7 +6953,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>632</v>
       </c>
@@ -6944,7 +6979,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>633</v>
       </c>
@@ -6970,7 +7005,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>634</v>
       </c>
@@ -6996,7 +7031,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>635</v>
       </c>
@@ -7022,7 +7057,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>636</v>
       </c>
@@ -7048,7 +7083,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>637</v>
       </c>
@@ -7074,7 +7109,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>638</v>
       </c>
@@ -7100,7 +7135,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>639</v>
       </c>
@@ -7126,7 +7161,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>640</v>
       </c>
@@ -7152,7 +7187,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>641</v>
       </c>
@@ -7178,7 +7213,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>642</v>
       </c>
@@ -7204,7 +7239,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>643</v>
       </c>
@@ -7230,7 +7265,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>644</v>
       </c>
@@ -7256,7 +7291,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>645</v>
       </c>
@@ -7282,7 +7317,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>646</v>
       </c>
@@ -7308,7 +7343,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>647</v>
       </c>
@@ -7334,7 +7369,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>648</v>
       </c>
@@ -7360,7 +7395,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>649</v>
       </c>
@@ -7386,7 +7421,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>650</v>
       </c>
@@ -7412,7 +7447,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>651</v>
       </c>
@@ -7438,7 +7473,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>652</v>
       </c>
@@ -7464,7 +7499,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="197" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>653</v>
       </c>
@@ -7490,7 +7525,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>654</v>
       </c>
@@ -7516,7 +7551,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>655</v>
       </c>
@@ -7542,7 +7577,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>656</v>
       </c>
@@ -7568,7 +7603,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>657</v>
       </c>
@@ -7594,7 +7629,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A202">
         <v>658</v>
       </c>
@@ -7620,7 +7655,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="203" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>659</v>
       </c>
@@ -7646,7 +7681,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="204" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A204">
         <v>660</v>
       </c>
@@ -7672,7 +7707,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="205" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A205">
         <v>661</v>
       </c>
@@ -7698,7 +7733,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="206" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A206">
         <v>662</v>
       </c>
@@ -7724,7 +7759,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A207">
         <v>663</v>
       </c>
@@ -7750,7 +7785,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="208" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A208">
         <v>664</v>
       </c>
@@ -7776,7 +7811,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="209" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A209">
         <v>665</v>
       </c>
@@ -7802,7 +7837,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="210" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A210">
         <v>666</v>
       </c>
@@ -7828,7 +7863,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="211" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A211">
         <v>667</v>
       </c>
@@ -7854,7 +7889,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="212" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A212">
         <v>668</v>
       </c>
@@ -7874,13 +7909,13 @@
         <v>11</v>
       </c>
       <c r="G212" s="1" t="s">
-        <v>36</v>
+        <v>660</v>
       </c>
       <c r="H212" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="213" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A213">
         <v>669</v>
       </c>
@@ -7906,7 +7941,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="214" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A214">
         <v>670</v>
       </c>
@@ -7932,7 +7967,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="215" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A215">
         <v>671</v>
       </c>
@@ -7958,7 +7993,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="216" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A216">
         <v>672</v>
       </c>
@@ -7984,7 +8019,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="217" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A217">
         <v>673</v>
       </c>
@@ -8010,7 +8045,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="218" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A218">
         <v>674</v>
       </c>
@@ -8036,7 +8071,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="219" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A219">
         <v>675</v>
       </c>
@@ -8062,7 +8097,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="220" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A220">
         <v>676</v>
       </c>
@@ -8082,13 +8117,13 @@
         <v>11</v>
       </c>
       <c r="G220" s="1" t="s">
-        <v>36</v>
+        <v>660</v>
       </c>
       <c r="H220" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="221" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A221">
         <v>677</v>
       </c>
@@ -8114,7 +8149,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="222" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A222">
         <v>678</v>
       </c>
@@ -8140,7 +8175,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="223" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A223">
         <v>679</v>
       </c>
@@ -8166,7 +8201,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="224" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A224">
         <v>680</v>
       </c>
@@ -8192,7 +8227,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="225" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A225">
         <v>681</v>
       </c>
@@ -8218,7 +8253,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="226" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A226">
         <v>682</v>
       </c>
@@ -8244,7 +8279,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="227" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A227">
         <v>683</v>
       </c>
@@ -8270,7 +8305,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="228" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A228">
         <v>684</v>
       </c>
@@ -8296,7 +8331,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="229" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A229">
         <v>685</v>
       </c>
@@ -8322,7 +8357,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="230" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A230">
         <v>686</v>
       </c>
@@ -8348,7 +8383,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="231" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A231">
         <v>687</v>
       </c>
@@ -8374,7 +8409,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="232" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A232">
         <v>688</v>
       </c>
@@ -8400,7 +8435,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="233" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A233">
         <v>689</v>
       </c>
@@ -8426,7 +8461,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="234" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A234">
         <v>690</v>
       </c>
@@ -8452,7 +8487,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="235" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A235">
         <v>691</v>
       </c>
@@ -8478,7 +8513,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="236" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A236">
         <v>692</v>
       </c>
@@ -8504,7 +8539,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="237" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A237">
         <v>693</v>
       </c>
@@ -8530,7 +8565,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="238" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A238">
         <v>694</v>
       </c>
@@ -8556,7 +8591,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="239" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A239">
         <v>695</v>
       </c>
@@ -8582,7 +8617,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="240" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A240">
         <v>696</v>
       </c>
@@ -8608,7 +8643,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="241" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A241">
         <v>697</v>
       </c>
@@ -8634,7 +8669,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="242" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A242">
         <v>698</v>
       </c>
@@ -8654,13 +8689,13 @@
         <v>11</v>
       </c>
       <c r="G242" s="1" t="s">
-        <v>36</v>
+        <v>659</v>
       </c>
       <c r="H242" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="243" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A243">
         <v>699</v>
       </c>
@@ -8686,7 +8721,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="244" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A244">
         <v>700</v>
       </c>
@@ -8712,7 +8747,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="245" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A245">
         <v>701</v>
       </c>
@@ -8738,7 +8773,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="246" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A246">
         <v>702</v>
       </c>
@@ -8764,7 +8799,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="247" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A247">
         <v>703</v>
       </c>
@@ -8790,7 +8825,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="248" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A248">
         <v>704</v>
       </c>
@@ -8816,7 +8851,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="249" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A249">
         <v>705</v>
       </c>
@@ -8842,7 +8877,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="250" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A250">
         <v>706</v>
       </c>
@@ -8868,7 +8903,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="251" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A251">
         <v>707</v>
       </c>
@@ -8894,7 +8929,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="252" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A252">
         <v>708</v>
       </c>
@@ -8914,13 +8949,13 @@
         <v>11</v>
       </c>
       <c r="G252" s="1" t="s">
-        <v>36</v>
+        <v>654</v>
       </c>
       <c r="H252" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="253" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A253">
         <v>709</v>
       </c>
@@ -8946,7 +8981,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="254" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A254">
         <v>710</v>
       </c>
@@ -8972,7 +9007,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="255" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A255">
         <v>711</v>
       </c>
@@ -8992,13 +9027,13 @@
         <v>11</v>
       </c>
       <c r="G255" s="1" t="s">
-        <v>36</v>
+        <v>657</v>
       </c>
       <c r="H255" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="256" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A256">
         <v>712</v>
       </c>
@@ -9024,7 +9059,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="257" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A257">
         <v>713</v>
       </c>
@@ -9050,7 +9085,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="258" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A258">
         <v>714</v>
       </c>
@@ -9070,13 +9105,13 @@
         <v>11</v>
       </c>
       <c r="G258" s="1" t="s">
-        <v>36</v>
+        <v>657</v>
       </c>
       <c r="H258" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="259" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A259">
         <v>715</v>
       </c>
@@ -9102,7 +9137,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="260" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A260">
         <v>716</v>
       </c>
@@ -9128,7 +9163,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="261" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A261">
         <v>717</v>
       </c>
@@ -9154,7 +9189,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="262" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A262">
         <v>718</v>
       </c>
@@ -9180,7 +9215,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="263" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A263">
         <v>719</v>
       </c>
@@ -9206,7 +9241,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="264" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A264">
         <v>720</v>
       </c>
@@ -9232,7 +9267,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="265" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A265">
         <v>721</v>
       </c>
@@ -9258,7 +9293,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="266" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A266">
         <v>722</v>
       </c>
@@ -9284,7 +9319,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="267" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A267">
         <v>723</v>
       </c>
@@ -9310,7 +9345,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="268" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A268">
         <v>724</v>
       </c>
@@ -9336,7 +9371,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="269" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A269">
         <v>725</v>
       </c>
@@ -9362,7 +9397,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="270" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A270">
         <v>726</v>
       </c>
@@ -9388,7 +9423,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="271" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A271">
         <v>727</v>
       </c>
@@ -9414,7 +9449,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="272" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A272">
         <v>728</v>
       </c>
@@ -9440,7 +9475,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="273" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A273">
         <v>729</v>
       </c>
@@ -9466,7 +9501,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="274" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A274">
         <v>730</v>
       </c>
@@ -9492,7 +9527,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="275" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A275">
         <v>731</v>
       </c>
@@ -9518,7 +9553,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="276" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A276">
         <v>732</v>
       </c>
@@ -9544,7 +9579,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="277" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A277">
         <v>733</v>
       </c>
@@ -9570,7 +9605,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="278" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A278">
         <v>734</v>
       </c>
@@ -9596,7 +9631,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="279" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A279">
         <v>735</v>
       </c>
@@ -9622,7 +9657,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="280" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A280">
         <v>736</v>
       </c>
@@ -9648,7 +9683,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="281" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A281">
         <v>737</v>
       </c>
@@ -9674,7 +9709,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="282" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A282">
         <v>738</v>
       </c>
@@ -9700,7 +9735,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="283" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A283">
         <v>739</v>
       </c>
@@ -9720,13 +9755,13 @@
         <v>11</v>
       </c>
       <c r="G283" s="1" t="s">
-        <v>36</v>
+        <v>660</v>
       </c>
       <c r="H283" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="284" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A284">
         <v>740</v>
       </c>
@@ -9752,7 +9787,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="285" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A285">
         <v>741</v>
       </c>
@@ -9778,7 +9813,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="286" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A286">
         <v>742</v>
       </c>
@@ -9804,7 +9839,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="287" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A287">
         <v>743</v>
       </c>
@@ -9830,7 +9865,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="288" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A288">
         <v>744</v>
       </c>
@@ -9856,7 +9891,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="289" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A289">
         <v>745</v>
       </c>
@@ -9882,7 +9917,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="290" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A290">
         <v>746</v>
       </c>
@@ -9908,7 +9943,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="291" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A291">
         <v>747</v>
       </c>
@@ -9934,7 +9969,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="292" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A292">
         <v>748</v>
       </c>
@@ -9954,13 +9989,13 @@
         <v>206</v>
       </c>
       <c r="G292" s="1" t="s">
-        <v>36</v>
+        <v>661</v>
       </c>
       <c r="H292" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="293" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A293">
         <v>749</v>
       </c>
@@ -9986,7 +10021,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="294" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A294">
         <v>750</v>
       </c>
@@ -10012,7 +10047,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="295" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A295">
         <v>751</v>
       </c>
@@ -10038,7 +10073,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="296" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A296">
         <v>752</v>
       </c>
@@ -10064,7 +10099,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="297" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A297">
         <v>753</v>
       </c>
@@ -10090,7 +10125,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="298" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A298">
         <v>754</v>
       </c>
@@ -10116,7 +10151,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="299" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A299">
         <v>755</v>
       </c>
@@ -10142,7 +10177,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="300" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A300">
         <v>756</v>
       </c>
@@ -10168,7 +10203,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="301" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A301">
         <v>757</v>
       </c>
@@ -10194,7 +10229,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="302" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A302">
         <v>758</v>
       </c>
@@ -10220,7 +10255,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="303" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A303">
         <v>759</v>
       </c>
@@ -10246,7 +10281,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="304" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A304">
         <v>760</v>
       </c>
@@ -10272,7 +10307,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="305" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A305">
         <v>761</v>
       </c>
@@ -10298,7 +10333,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="306" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A306">
         <v>762</v>
       </c>
@@ -10324,7 +10359,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="307" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A307">
         <v>763</v>
       </c>
@@ -10350,7 +10385,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="308" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A308">
         <v>764</v>
       </c>
@@ -10376,7 +10411,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="309" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A309">
         <v>765</v>
       </c>
@@ -10402,7 +10437,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="310" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A310">
         <v>766</v>
       </c>
@@ -10428,7 +10463,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="311" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A311">
         <v>767</v>
       </c>
@@ -10454,7 +10489,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="312" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A312">
         <v>768</v>
       </c>
@@ -10480,7 +10515,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="313" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A313">
         <v>769</v>
       </c>
@@ -10500,13 +10535,13 @@
         <v>11</v>
       </c>
       <c r="G313" s="1" t="s">
-        <v>36</v>
+        <v>654</v>
       </c>
       <c r="H313" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="314" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A314">
         <v>770</v>
       </c>
@@ -10532,7 +10567,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="315" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A315">
         <v>771</v>
       </c>
@@ -10558,7 +10593,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="316" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A316">
         <v>772</v>
       </c>
@@ -10584,7 +10619,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="317" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A317">
         <v>773</v>
       </c>
@@ -10610,7 +10645,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="318" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A318">
         <v>774</v>
       </c>
@@ -10636,7 +10671,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="319" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A319">
         <v>775</v>
       </c>
@@ -10656,13 +10691,13 @@
         <v>11</v>
       </c>
       <c r="G319" s="1" t="s">
-        <v>36</v>
+        <v>654</v>
       </c>
       <c r="H319" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="320" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A320">
         <v>776</v>
       </c>
@@ -10682,13 +10717,13 @@
         <v>11</v>
       </c>
       <c r="G320" s="1" t="s">
-        <v>36</v>
+        <v>654</v>
       </c>
       <c r="H320" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="321" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A321">
         <v>777</v>
       </c>
@@ -10708,13 +10743,13 @@
         <v>11</v>
       </c>
       <c r="G321" s="1" t="s">
-        <v>36</v>
+        <v>654</v>
       </c>
       <c r="H321" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="322" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A322">
         <v>778</v>
       </c>
@@ -10740,7 +10775,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="323" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A323">
         <v>779</v>
       </c>
@@ -10766,7 +10801,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="324" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A324">
         <v>780</v>
       </c>
@@ -10792,7 +10827,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="325" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A325">
         <v>781</v>
       </c>
@@ -10818,7 +10853,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="326" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A326">
         <v>782</v>
       </c>
@@ -10844,7 +10879,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="327" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A327">
         <v>783</v>
       </c>
@@ -10870,7 +10905,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="328" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A328">
         <v>784</v>
       </c>
@@ -10896,7 +10931,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="329" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A329">
         <v>785</v>
       </c>
@@ -10922,7 +10957,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="330" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A330">
         <v>786</v>
       </c>
@@ -10948,7 +10983,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="331" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A331">
         <v>787</v>
       </c>
@@ -10974,7 +11009,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="332" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A332">
         <v>788</v>
       </c>
@@ -11000,7 +11035,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="333" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A333">
         <v>789</v>
       </c>
@@ -11026,7 +11061,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="334" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A334">
         <v>790</v>
       </c>
@@ -11052,7 +11087,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="335" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A335">
         <v>791</v>
       </c>
@@ -11072,13 +11107,13 @@
         <v>206</v>
       </c>
       <c r="G335" s="1" t="s">
-        <v>36</v>
+        <v>655</v>
       </c>
       <c r="H335" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="336" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A336">
         <v>792</v>
       </c>
@@ -11104,7 +11139,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="337" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A337">
         <v>793</v>
       </c>
@@ -11130,7 +11165,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="338" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A338">
         <v>794</v>
       </c>
@@ -11156,7 +11191,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="339" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A339">
         <v>795</v>
       </c>
@@ -11182,7 +11217,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="340" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A340">
         <v>796</v>
       </c>
@@ -11202,13 +11237,13 @@
         <v>11</v>
       </c>
       <c r="G340" s="1" t="s">
-        <v>36</v>
+        <v>660</v>
       </c>
       <c r="H340" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="341" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A341">
         <v>797</v>
       </c>
@@ -11228,13 +11263,13 @@
         <v>11</v>
       </c>
       <c r="G341" s="1" t="s">
-        <v>36</v>
+        <v>654</v>
       </c>
       <c r="H341" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="342" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A342">
         <v>798</v>
       </c>
@@ -11260,7 +11295,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="343" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A343">
         <v>799</v>
       </c>
@@ -11286,7 +11321,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="344" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A344">
         <v>800</v>
       </c>
@@ -11312,7 +11347,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="345" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A345">
         <v>801</v>
       </c>
@@ -11338,7 +11373,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="346" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A346">
         <v>802</v>
       </c>
@@ -11364,7 +11399,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="347" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A347">
         <v>803</v>
       </c>
@@ -11390,7 +11425,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="348" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A348">
         <v>804</v>
       </c>
@@ -11416,7 +11451,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="349" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A349">
         <v>805</v>
       </c>
@@ -11442,7 +11477,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="350" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A350">
         <v>806</v>
       </c>
@@ -11468,7 +11503,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="351" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A351">
         <v>807</v>
       </c>
@@ -11494,7 +11529,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="352" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A352">
         <v>808</v>
       </c>
@@ -11520,7 +11555,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="353" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A353">
         <v>809</v>
       </c>
@@ -11546,7 +11581,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="354" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A354">
         <v>810</v>
       </c>
@@ -11572,7 +11607,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="355" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A355">
         <v>811</v>
       </c>
@@ -11598,7 +11633,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="356" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A356">
         <v>812</v>
       </c>
@@ -11624,7 +11659,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="357" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A357">
         <v>813</v>
       </c>
@@ -11650,7 +11685,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="358" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A358">
         <v>814</v>
       </c>
@@ -11676,7 +11711,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="359" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A359">
         <v>815</v>
       </c>
@@ -11702,7 +11737,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="360" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A360">
         <v>816</v>
       </c>
@@ -11728,7 +11763,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="361" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A361">
         <v>817</v>
       </c>
@@ -11754,7 +11789,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="362" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A362">
         <v>818</v>
       </c>
@@ -11780,7 +11815,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="363" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A363">
         <v>819</v>
       </c>
@@ -11806,7 +11841,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="364" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A364">
         <v>820</v>
       </c>
@@ -11832,7 +11867,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="365" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A365">
         <v>821</v>
       </c>
@@ -11858,7 +11893,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="366" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A366">
         <v>822</v>
       </c>
@@ -11884,7 +11919,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="367" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A367">
         <v>823</v>
       </c>
@@ -11910,7 +11945,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="368" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A368">
         <v>824</v>
       </c>
@@ -11936,7 +11971,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="369" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A369">
         <v>825</v>
       </c>
@@ -11962,7 +11997,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="370" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A370">
         <v>826</v>
       </c>
@@ -11988,7 +12023,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="371" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A371">
         <v>827</v>
       </c>
@@ -12014,7 +12049,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="372" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A372">
         <v>828</v>
       </c>
@@ -12040,7 +12075,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="373" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A373">
         <v>829</v>
       </c>
@@ -12066,7 +12101,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="374" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A374">
         <v>830</v>
       </c>
@@ -12092,7 +12127,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="375" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A375">
         <v>831</v>
       </c>
@@ -12118,7 +12153,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="376" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A376">
         <v>832</v>
       </c>
@@ -12144,7 +12179,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="377" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A377">
         <v>833</v>
       </c>
@@ -12170,7 +12205,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="378" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A378">
         <v>834</v>
       </c>
@@ -12196,7 +12231,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="379" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A379">
         <v>835</v>
       </c>
@@ -12222,7 +12257,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="380" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A380">
         <v>836</v>
       </c>
@@ -12248,7 +12283,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="381" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A381">
         <v>837</v>
       </c>
@@ -12274,7 +12309,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="382" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A382">
         <v>838</v>
       </c>
@@ -12300,7 +12335,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="383" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A383">
         <v>839</v>
       </c>
@@ -12326,7 +12361,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="384" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A384">
         <v>840</v>
       </c>
@@ -12352,7 +12387,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="385" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A385">
         <v>841</v>
       </c>
@@ -12378,7 +12413,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="386" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A386">
         <v>842</v>
       </c>
@@ -12404,7 +12439,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="387" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="387" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A387">
         <v>843</v>
       </c>
@@ -12430,7 +12465,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="388" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A388">
         <v>844</v>
       </c>
@@ -12456,7 +12491,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="389" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="389" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A389">
         <v>845</v>
       </c>
@@ -12482,7 +12517,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="390" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="390" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A390">
         <v>846</v>
       </c>
@@ -12508,7 +12543,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="391" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="391" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A391">
         <v>847</v>
       </c>
@@ -12534,7 +12569,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="392" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="392" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A392">
         <v>848</v>
       </c>
@@ -12560,7 +12595,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="393" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="393" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A393">
         <v>849</v>
       </c>
@@ -12586,7 +12621,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="394" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="394" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A394">
         <v>850</v>
       </c>
@@ -12612,7 +12647,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="395" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="395" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A395">
         <v>851</v>
       </c>
@@ -12638,7 +12673,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="396" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="396" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A396">
         <v>852</v>
       </c>
@@ -12664,7 +12699,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="397" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="397" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A397">
         <v>853</v>
       </c>
@@ -12690,7 +12725,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="398" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="398" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A398">
         <v>854</v>
       </c>
@@ -12716,7 +12751,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="399" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="399" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A399">
         <v>855</v>
       </c>
@@ -12742,7 +12777,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="400" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="400" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A400">
         <v>856</v>
       </c>
@@ -12768,7 +12803,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="401" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="401" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A401">
         <v>857</v>
       </c>
@@ -12794,7 +12829,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="402" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="402" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A402">
         <v>858</v>
       </c>
@@ -12820,7 +12855,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="403" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="403" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A403">
         <v>859</v>
       </c>
@@ -12846,7 +12881,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="404" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="404" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A404">
         <v>860</v>
       </c>
@@ -12872,7 +12907,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="405" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="405" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A405">
         <v>861</v>
       </c>
@@ -12898,7 +12933,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="406" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="406" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A406">
         <v>862</v>
       </c>
@@ -12924,7 +12959,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="407" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="407" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A407">
         <v>863</v>
       </c>
@@ -12950,7 +12985,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="408" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="408" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A408">
         <v>864</v>
       </c>
@@ -12976,7 +13011,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="409" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="409" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A409">
         <v>865</v>
       </c>
@@ -13002,7 +13037,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="410" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="410" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A410">
         <v>866</v>
       </c>
@@ -13028,7 +13063,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="411" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="411" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A411">
         <v>867</v>
       </c>
@@ -13054,7 +13089,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="412" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="412" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A412">
         <v>868</v>
       </c>
@@ -13080,7 +13115,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="413" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="413" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A413">
         <v>869</v>
       </c>
@@ -13106,7 +13141,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="414" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="414" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A414">
         <v>870</v>
       </c>
@@ -13132,7 +13167,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="415" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="415" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A415">
         <v>871</v>
       </c>
@@ -13158,7 +13193,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="416" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="416" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A416">
         <v>872</v>
       </c>
@@ -13184,7 +13219,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="417" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="417" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A417">
         <v>873</v>
       </c>
@@ -13210,7 +13245,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="418" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="418" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A418">
         <v>874</v>
       </c>
@@ -13236,7 +13271,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="419" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="419" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A419">
         <v>875</v>
       </c>
@@ -13262,7 +13297,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="420" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="420" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A420">
         <v>876</v>
       </c>
@@ -13288,7 +13323,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="421" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="421" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A421">
         <v>877</v>
       </c>
@@ -13314,7 +13349,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="422" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="422" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A422">
         <v>878</v>
       </c>
@@ -13340,7 +13375,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="423" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="423" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A423">
         <v>879</v>
       </c>
@@ -13360,13 +13395,13 @@
         <v>35</v>
       </c>
       <c r="G423" s="1" t="s">
-        <v>36</v>
+        <v>662</v>
       </c>
       <c r="H423" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="424" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="424" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A424">
         <v>880</v>
       </c>
@@ -13392,7 +13427,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="425" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="425" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A425">
         <v>881</v>
       </c>
@@ -13418,7 +13453,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="426" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="426" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A426">
         <v>882</v>
       </c>
@@ -13444,7 +13479,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="427" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="427" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A427">
         <v>883</v>
       </c>
@@ -13470,7 +13505,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="428" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="428" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A428">
         <v>884</v>
       </c>
@@ -13496,7 +13531,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="429" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="429" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A429">
         <v>885</v>
       </c>
@@ -13522,7 +13557,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="430" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="430" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A430">
         <v>886</v>
       </c>
@@ -13548,7 +13583,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="431" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="431" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A431">
         <v>887</v>
       </c>
@@ -13574,7 +13609,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="432" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="432" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A432">
         <v>888</v>
       </c>
@@ -13600,7 +13635,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="433" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="433" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A433">
         <v>889</v>
       </c>
@@ -13626,7 +13661,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="434" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="434" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A434">
         <v>890</v>
       </c>
@@ -13652,7 +13687,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="435" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="435" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A435">
         <v>891</v>
       </c>
@@ -13672,13 +13707,13 @@
         <v>11</v>
       </c>
       <c r="G435" s="1" t="s">
-        <v>36</v>
+        <v>663</v>
       </c>
       <c r="H435" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="436" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="436" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A436">
         <v>892</v>
       </c>
@@ -13704,7 +13739,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="437" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="437" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A437">
         <v>893</v>
       </c>
@@ -13730,7 +13765,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="438" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="438" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A438">
         <v>894</v>
       </c>
@@ -13750,13 +13785,13 @@
         <v>11</v>
       </c>
       <c r="G438" s="1" t="s">
-        <v>36</v>
+        <v>663</v>
       </c>
       <c r="H438" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="439" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="439" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A439">
         <v>895</v>
       </c>
@@ -13782,7 +13817,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="440" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="440" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A440">
         <v>896</v>
       </c>
@@ -13808,7 +13843,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="441" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="441" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A441">
         <v>897</v>
       </c>
@@ -13834,7 +13869,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="442" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="442" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A442">
         <v>898</v>
       </c>
@@ -13860,7 +13895,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="443" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="443" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A443">
         <v>899</v>
       </c>
@@ -13886,7 +13921,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="444" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="444" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A444">
         <v>900</v>
       </c>
@@ -13906,13 +13941,13 @@
         <v>11</v>
       </c>
       <c r="G444" s="1" t="s">
-        <v>36</v>
+        <v>663</v>
       </c>
       <c r="H444" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="445" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="445" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A445">
         <v>901</v>
       </c>
@@ -13938,7 +13973,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="446" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="446" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A446">
         <v>902</v>
       </c>
@@ -13964,7 +13999,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="447" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="447" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A447">
         <v>903</v>
       </c>

</xml_diff>